<commit_message>
edit to blue bike tutorial
</commit_message>
<xml_diff>
--- a/docs/Tutorial/img/BlueBikesDataPortal.xlsx
+++ b/docs/Tutorial/img/BlueBikesDataPortal.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\compo\Documents\DocumentationFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\ComposableDocs\Docs\docs\Tutorial\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C498224-45F5-4438-A681-ACCC0261EDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD9A984-9561-40FB-9273-4A618AC6A3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="360" windowWidth="28770" windowHeight="15060" tabRatio="935" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Master" sheetId="24" r:id="rId1"/>
-    <sheet name="Master.settings" sheetId="38" r:id="rId2"/>
-    <sheet name="BlueBikes" sheetId="37" r:id="rId3"/>
-    <sheet name="TripData" sheetId="2" r:id="rId4"/>
-    <sheet name="Categories" sheetId="36" r:id="rId5"/>
+    <sheet name="ReadMe" sheetId="39" r:id="rId1"/>
+    <sheet name="Master" sheetId="24" r:id="rId2"/>
+    <sheet name="Master.settings" sheetId="38" r:id="rId3"/>
+    <sheet name="BlueBikes" sheetId="37" r:id="rId4"/>
+    <sheet name="TripData" sheetId="2" r:id="rId5"/>
+    <sheet name="Categories" sheetId="36" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TripData!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TripData!$A$1:$E$1</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -219,7 +221,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,13 +242,34 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -261,13 +284,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -311,6 +336,2983 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19052</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>628651</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B6068DB-4454-40B7-B69B-87677D151C40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19052" y="19050"/>
+          <a:ext cx="8515349" cy="22029420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DataPortals ReadMe</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This Readme is a quick summary of all the options available in Composable DataPortals to customize your data models.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>For a more complete description, please review the docs at </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>https://docs.composable.ai</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Excel Workbook Sheet Structure</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Master</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:  This is the first sheet that is processed in this</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DataPortals Model File and acts as a link to all other container sheets that will ultimately be shown to the end user.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Master.settings: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(optional) The settings sheet allows for some customization of DataPortal actions. A settings sheet has two columns, Option and Value.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> S</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ettings defined in the Master.settings sheet will apply for the entire DataPortal.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>“</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Container</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>”:  These can be any name that is not reserved and specify what input fields are listed out in each web page the user sees, as well as any controlling logic of how they are saved and displayed.  In the server, each input field name represents a column in an SQL table.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>“</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Category</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>":  These specify a single picklist for the end user, such as Gender or State you live in.  They can be in its own sheet or in the Categories sheet.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Categories</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: On this sheet, each column represents its own category to simplify the excel structure if you have a lot of categories in your form.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ReadMe</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: This sheet is not processed or displayed to the end user of forms, it is a place to store notes and comments on the form. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>CSS</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:  An optional sheet to enter custom CSS rules to style the DataPortals web interface with any colors, margins or other style behavior. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Control Definitions</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Note</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Fields with an (*) are required to process a sheet.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Name</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:­­ This is the name of the variable that is saved in the database.  The name must be unique on the page and cannot be ID or the sheet name.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DisplayName</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: This is the name displayed to the end user as a label above the input field.  If left blank, the name field is used.  If “NoDisplayName” is used, the label is left blank.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Description</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: This is optional extra information displayed to the user if they hover over an info (i) icon above the input field.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Type</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:  This is the variable that the input field represents in the database.  There are three main types of values you can put in this field: system types, such as System.String; category types, which represent a sort of picklist; container types, which represent a link to another page or table if it’s a one to many relationships.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ControlType</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:  This field determines how the input field is displayed to the end user and must match the type on the backend.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>AppRun</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Specifies a button that runs a Composable DataFlow Application given the DataFlow's AppID.  Not an input type. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Boolean</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Checkbox for Boolean types.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Category</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Picklist for Category types.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DateTime</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: UI picker for a date type.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Decimal</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Decimal input field.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Integer</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Integer input field.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Label</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: A string input that can be styled by having the DisplayName be processed as markdown. Not an input type.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>MultiCategory</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Picklist Category types where multiple selections can be made. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Page</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Link to a signle child Container types. Not an input type.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Spin</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Supported for numeric types, offers a spin clicker UI for cycling through valid numbers. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SSN</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Only allows valid SSN entries to be saved. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>String</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: String input field.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Tab</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Specifies a tab to be displayed on the page to control visibility between items. Not an input type.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Table</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: A link to many of the same child Container types.  New child containers can be created, but otherwise not an input type.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Textarea</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Larger string input field.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Telephone</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Only allows valid telephone entries to be saved.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Voice</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Experimental, a Larger string input field that allows voice input.  Only supported in Chrome.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Columns</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Only processed for the Table ControlType.  Specifies what columns in the child sheets appear in the table for the user.  Using JSON notation, have the option to rename the column names from their defaults.  If left blank, only each record ID is shown in the table.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SearchBoxes</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:  Only processed for the Table ControlType.  If value is “True”, a search box appears below each column header in the Table.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Min</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:  Only processed for numeric or date-time types, defines a lower bound on the value that can be stored in the database.  A warning is given to the user if the input is invalid.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Max</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Only processed for numeric or date-time types, defines an upper bound on the value that can be stored in the database.  A warning is given to the user if the input is invalid.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>StrMin</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Only processed for System.String, defines a lower bound on the number of characters that can be stored in the database. A default value satisfying this min length must be provided to use this field. A warning is given to the user if the input is invalid.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>StrMax</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Only processed for System.String, defines an upper bound on the number of characters that can be stored in the database.  A warning is given to the user if the input is invalid.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>VisibilityCondition</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Checks the value of another input field on the page to see if this field is displayed to the user.  Supports Boolean logic ANDs (&amp;&amp;), ORs (||) and parenthesis.  If the check returns false, the input is not displayed to the user. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>MaskedCondition</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Checks the value of another input field on the page to see if this field is displayed to the user like visibility condition, but instead of not displayed the item, masks the item and shows white space where the input field normally is</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>OptionController</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Uses a pipe separated list to determine visibility conditions for a category controlType.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ReadOnlyCondition</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Processed on all input types.  If set to “True”, the input field is grayed out and only data prepopulated in forms will be displayed.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DeleteType</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Only processed for containers. If set to “Soft”, the record is still saved in the database on delete.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DefaultValue</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:  Processed on all input types, sets the value that the user first sees. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Required</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Processed on all input types.  If set to “True”, a user must supply a value for the page to be saved.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Group</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Processed on everything displayed on the screen, specifying which group &lt;div&gt; it is displayed within.  Groups are processed top-down.  Nesting of items in a group is achieved with separating group names with a “.” while horizontally laying out elements in a div is achieved by ending the group names with H or HC for horizontal and horizontally centered respectively.  Ending a group name with T and a digit 1-12 will place the field in a horizontal row, always taking up increments of 1/12 of the width of the page.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ControlGroup</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Only processed for the Tab Control Type.  Specifies which group in the Group column is displayed when the tab is selected.  Overrides visibility conditions.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Group layout example:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>First, you don’t need to give any field a group. If you omit groups, fields will display vertically stacked on the page, each filling 100% of the width of the page.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The group column takes in a group name with no spaces.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Groups are arranged in a hierarchy by dot notation. “Cars.Chevy” puts a field in the “Cars” group, and in the “Chevy” subgroup inside of “Cars”.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A colored (light grey) background is displayed under each top-level group. If fields exist inside the “Cars” group and a “Trains” group, those groups will be visually separated on the page with gaps between their respective grey background areas.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Groups are stacked one below the other, vertically, on the page. The order of the groups is determined by the respective ordering in the Excel of the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>first field in a given group</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The most common way of laying out the form is by setting up groups of fields to be displayed horizontally next to each other across the page. We support a suffix notation to specify the widths of fields to support displaying a row of fields horizontally across the page. To have a field take up less than the full width of the page, append the letter “T” to the end of the group name, followed by a number between 1 and 12, representing the fraction of the page you’d like the field to fill. (“T6” is half the page, “T1” is 1/12 of the page).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="457200" marR="0" lvl="1" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Since this is the most common structure, I’ll show an example.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="457200" marR="0" lvl="1" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Let’s put all of our fields into a top-level group, so that all of the fields will be displayed in the same light grey box on the page. We’ll call this group “A”.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="457200" marR="0" lvl="1" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Let’s say we have 6 fields to display on the page, with the following layout: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="914400" marR="0" lvl="2" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The first field on its own across the top of the page, taking up the full width.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="914400" marR="0" lvl="2" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Fields 2-3 below field 1, next to each other horizontally, each taking up half of the width of the page.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="914400" marR="0" lvl="2" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Fields 4-6 below fields 2-3, next to each other horizontally, each taking up a third of the width of the page.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="914400" marR="0" lvl="2" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>To achieve this, we’d assign the following groups to the fields:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1371600" marR="0" lvl="3" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Field 1: “A.FirstRow”</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1828800" marR="0" lvl="4" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The form will create a group called “A”, then a group called “FirstRow” inside of it. As no width was specified, this field will fill the full width of the page.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1371600" marR="0" lvl="3" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Field 2: “A.SecondRowT6”</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1828800" marR="0" lvl="4" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The form will create a new group called “SecondRow” inside the existing group “A”, which will be displayed below the “FirstRow” group. This field will take up half of the width of the page (due to the “T6” suffix), aligned to the left of the new “SecondRow”. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1371600" marR="0" lvl="3" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Field 3: “A.SecondRowT6”</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1828800" marR="0" lvl="4" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The form will insert this field into the “SecondRow” group, where it will take up the remaining half of the page width, to the right of Field 2.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1371600" marR="0" lvl="3" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Field 4: “A.ThirdRowT4”</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1828800" marR="0" lvl="4" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The form will create a new group “ThirdRow” inside top-level group “A”, which will appear below the “SecondRow” group on the page. This field will be displayed on the left side of the “ThirdRow” group and will take up 4/12 = one third of the width of the page.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1371600" marR="0" lvl="3" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Field 5: “A.ThirdRowT4”</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1828800" marR="0" lvl="4" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The form will place this field inside the “ThirdRow” group, to the right of Field 4, taking up the middle third of the page horizontally.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1371600" marR="0" lvl="3" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Field 6: “A.ThirdRowT4”</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="1828800" marR="0" lvl="4" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The form will place this field inside the “ThirdRow” group, to the right of Field 5, taking up the right third of the page horizontally.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -609,11 +3611,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FEBF711-49E9-4258-A401-328D5E203592}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:E2"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -627,19 +3648,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -655,6 +3676,41 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F6FCF7-B437-4DCE-9C13-D3E40C81062C}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -662,75 +3718,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F6FCF7-B437-4DCE-9C13-D3E40C81062C}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F1253F-71D2-449C-A8F8-9C34628B96D9}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -798,42 +3827,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1039,8 +4071,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1054,7 +4089,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>